<commit_message>
Pruebas adicionales en windows
</commit_message>
<xml_diff>
--- a/task-processor-performance/datos/Graficos.xlsx
+++ b/task-processor-performance/datos/Graficos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="9780"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="9570" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Ejecucion mas rápida" sheetId="1" r:id="rId1"/>
@@ -478,7 +478,7 @@
   <dimension ref="A2:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,8 +535,12 @@
       <c r="C5" s="3">
         <v>0</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -545,7 +549,10 @@
       <c r="B6" s="3">
         <v>914424</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3">
+        <f xml:space="preserve"> 8 * 20127.75</f>
+        <v>161022</v>
+      </c>
       <c r="D6" s="3">
         <f>8 * 589630.29</f>
         <v>4717042.32</v>
@@ -560,9 +567,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>858732</v>
-      </c>
-      <c r="C7" s="3"/>
+        <f>4 * 194176.23</f>
+        <v>776704.92</v>
+      </c>
+      <c r="C7" s="3">
+        <f>4 * 37921.61</f>
+        <v>151686.44</v>
+      </c>
       <c r="D7" s="3">
         <f xml:space="preserve"> 4 *944117.5</f>
         <v>3776470</v>
@@ -577,9 +588,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="3">
-        <v>495782.83</v>
-      </c>
-      <c r="C8" s="3"/>
+        <f>4*125486.01</f>
+        <v>501944.04</v>
+      </c>
+      <c r="C8" s="3">
+        <f>4 * 38627.17</f>
+        <v>154508.68</v>
+      </c>
       <c r="D8" s="3">
         <f>4 * 466324.96</f>
         <v>1865299.84</v>
@@ -594,9 +609,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="3">
-        <v>250016.08</v>
-      </c>
-      <c r="C9" s="3"/>
+        <f>2*125605.79</f>
+        <v>251211.58</v>
+      </c>
+      <c r="C9" s="3">
+        <f>2 * 39277.56</f>
+        <v>78555.12</v>
+      </c>
       <c r="D9" s="3">
         <f>2*489983.22</f>
         <v>979966.44</v>
@@ -611,9 +630,11 @@
         <v>3</v>
       </c>
       <c r="B10" s="3">
-        <v>217192.32000000001</v>
-      </c>
-      <c r="C10" s="3"/>
+        <v>194494.19</v>
+      </c>
+      <c r="C10" s="3">
+        <v>38212.33</v>
+      </c>
       <c r="D10" s="3">
         <v>498985.7</v>
       </c>
@@ -626,9 +647,11 @@
         <v>4</v>
       </c>
       <c r="B11" s="3">
-        <v>158334.75</v>
-      </c>
-      <c r="C11" s="3"/>
+        <v>156932.69</v>
+      </c>
+      <c r="C11" s="3">
+        <v>37754.9</v>
+      </c>
       <c r="D11" s="3">
         <v>1236722.81</v>
       </c>
@@ -641,10 +664,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="3">
-        <v>125630.57</v>
+        <v>126163.42</v>
       </c>
       <c r="C12" s="3">
-        <v>39197.279999999999</v>
+        <v>39294.65</v>
       </c>
       <c r="D12" s="3">
         <v>499195.16</v>
@@ -658,10 +681,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="3">
-        <v>19157.599999999999</v>
+        <v>9483.93</v>
       </c>
       <c r="C13" s="3">
-        <v>14442.32</v>
+        <v>10493.774600000001</v>
       </c>
       <c r="D13" s="3">
         <v>41216.58</v>
@@ -677,37 +700,49 @@
       <c r="B14" s="3">
         <v>6136.74</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3">
+        <v>5427.03</v>
+      </c>
       <c r="D14" s="3">
         <v>101510.56</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3">
+        <v>3703.44</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="3">
-        <v>3624.49</v>
+        <v>4774.7299999999996</v>
       </c>
       <c r="C15" s="3">
-        <v>2967.06</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+        <v>2509.35</v>
+      </c>
+      <c r="D15" s="3">
+        <v>14520.36</v>
+      </c>
+      <c r="E15" s="3">
+        <v>3334.15</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="3">
-        <v>1280.3900000000001</v>
+        <v>1075.8900000000001</v>
       </c>
       <c r="C16" s="3">
-        <v>3000.81</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+        <v>2508.8200000000002</v>
+      </c>
+      <c r="D16" s="3">
+        <v>8374.8700000000008</v>
+      </c>
+      <c r="E16" s="3">
+        <v>3108.3</v>
+      </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>

</xml_diff>

<commit_message>
Cambios para optimizar ejecuciones
</commit_message>
<xml_diff>
--- a/task-processor-performance/datos/Graficos.xlsx
+++ b/task-processor-performance/datos/Graficos.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Descripción de test</t>
   </si>
@@ -94,12 +94,6 @@
     <t>4VM x UnicoThreadALoBruto</t>
   </si>
   <si>
-    <t>Windows</t>
-  </si>
-  <si>
-    <t>Linux</t>
-  </si>
-  <si>
     <t>1 NoSync</t>
   </si>
   <si>
@@ -110,6 +104,15 @@
   </si>
   <si>
     <t>4 Sync</t>
+  </si>
+  <si>
+    <t>% Conc</t>
+  </si>
+  <si>
+    <t>IkariSrv02 (Linux64)</t>
+  </si>
+  <si>
+    <t>Ikari01 (windows32)</t>
   </si>
 </sst>
 </file>
@@ -166,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -174,6 +177,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -186,6 +193,1117 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-AR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR"/>
+              <a:t>Multi VM NoSync</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$B$3:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ikari01 (windows32)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$6:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SimpleLoopMultiThreadTester x 1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>UnicoThreadALoBruto</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$B$6:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>914424</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>776704.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>501944.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>251211.58</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>194494.19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>156932.69</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>126163.42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$E$3:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IkariSrv02 (Linux64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$6:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SimpleLoopMultiThreadTester x 1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>UnicoThreadALoBruto</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$E$6:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4717042.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3776470</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1865299.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>979966.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1237362.42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1234625.8999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>499195.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="44424576"/>
+        <c:axId val="78760192"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="44424576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="78760192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="78760192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="44424576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-AR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR"/>
+              <a:t>Multi VM Sync</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$B$3:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ikari01 (windows32)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$6:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SimpleLoopMultiThreadTester x 1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>UnicoThreadALoBruto</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$C$6:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>161022</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>151686.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>154508.68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78555.12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38212.33</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37754.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39294.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$E$3:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IkariSrv02 (Linux64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$6:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SimpleLoopMultiThreadTester x 1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>UnicoThreadALoBruto</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$F$6:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>247626.56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>242459.28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>165256.32000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>140628.66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>69191.94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67903.42</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>73167.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="38571392"/>
+        <c:axId val="85423232"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="38571392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="85423232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="85423232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="38571392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-AR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR"/>
+              <a:t>Multi Thread NoSync</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$B$3:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ikari01 (windows32)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$13:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MultiplesThreadsALoBruto x 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SimpleLoopMultiThreadTester x 4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MultiplesThreadsALoBruto x 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MultiplesThreadsALoBruto x 32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9483.93</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6136.74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4774.7299999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1075.8900000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$E$3:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IkariSrv02 (Linux64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$13:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MultiplesThreadsALoBruto x 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SimpleLoopMultiThreadTester x 4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MultiplesThreadsALoBruto x 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MultiplesThreadsALoBruto x 32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$E$13:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>41216.58</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101510.56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14520.36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8374.8700000000008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="85651840"/>
+        <c:axId val="85654528"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="85651840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="85654528"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="85654528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="85651840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-AR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR"/>
+              <a:t>Multi Thread Sync</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$B$3:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ikari01 (windows32)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$13:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MultiplesThreadsALoBruto x 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SimpleLoopMultiThreadTester x 4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MultiplesThreadsALoBruto x 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MultiplesThreadsALoBruto x 32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$C$13:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10493.774600000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5427.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2509.35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2508.8200000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$E$3:$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IkariSrv02 (Linux64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$13:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MultiplesThreadsALoBruto x 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SimpleLoopMultiThreadTester x 4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MultiplesThreadsALoBruto x 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MultiplesThreadsALoBruto x 32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$F$13:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6445.97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3703.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3334.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3108.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="85627264"/>
+        <c:axId val="85645184"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="85627264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="85645184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="85645184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="85627264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -475,10 +1593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E28"/>
+  <dimension ref="A2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,46 +1604,53 @@
     <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -535,14 +1660,15 @@
       <c r="C5" s="3">
         <v>0</v>
       </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
+      <c r="D5" s="3"/>
       <c r="E5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -553,16 +1679,24 @@
         <f xml:space="preserve"> 8 * 20127.75</f>
         <v>161022</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="6">
+        <f>C6/B6</f>
+        <v>0.17609117870922023</v>
+      </c>
+      <c r="E6" s="3">
         <f>8 * 589630.29</f>
         <v>4717042.32</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <f xml:space="preserve"> 8 *30953.32</f>
         <v>247626.56</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" s="6">
+        <f>F6/E6</f>
+        <v>5.2496149748344843E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -574,16 +1708,24 @@
         <f>4 * 37921.61</f>
         <v>151686.44</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
+        <f t="shared" ref="D7:D16" si="0">C7/B7</f>
+        <v>0.19529481028651138</v>
+      </c>
+      <c r="E7" s="3">
         <f xml:space="preserve"> 4 *944117.5</f>
         <v>3776470</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <f>4 * 60614.82</f>
         <v>242459.28</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" s="6">
+        <f t="shared" ref="G7:G16" si="1">F7/E7</f>
+        <v>6.4202623084520724E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -595,16 +1737,24 @@
         <f>4 * 38627.17</f>
         <v>154508.68</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.30782052915699526</v>
+      </c>
+      <c r="E8" s="3">
         <f>4 * 466324.96</f>
         <v>1865299.84</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <f>4 * 41314.08</f>
         <v>165256.32000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" s="6">
+        <f t="shared" si="1"/>
+        <v>8.8595043250526417E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -616,16 +1766,24 @@
         <f>2 * 39277.56</f>
         <v>78555.12</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="6">
+        <f t="shared" si="0"/>
+        <v>0.31270501144891488</v>
+      </c>
+      <c r="E9" s="3">
         <f>2*489983.22</f>
         <v>979966.44</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="3">
         <f xml:space="preserve"> 2 * 70314.33</f>
         <v>140628.66</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" s="6">
+        <f t="shared" si="1"/>
+        <v>0.14350354691738221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -635,14 +1793,22 @@
       <c r="C10" s="3">
         <v>38212.33</v>
       </c>
-      <c r="D10" s="3">
-        <v>498985.7</v>
+      <c r="D10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.19647029044929312</v>
       </c>
       <c r="E10" s="3">
+        <v>1237362.42</v>
+      </c>
+      <c r="F10" s="3">
         <v>69191.94</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10" s="6">
+        <f t="shared" si="1"/>
+        <v>5.5918895613461417E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -652,14 +1818,22 @@
       <c r="C11" s="3">
         <v>37754.9</v>
       </c>
-      <c r="D11" s="3">
-        <v>1236722.81</v>
+      <c r="D11" s="6">
+        <f t="shared" si="0"/>
+        <v>0.24058021308371125</v>
       </c>
       <c r="E11" s="3">
+        <v>1234625.8999999999</v>
+      </c>
+      <c r="F11" s="3">
         <v>67903.42</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11" s="6">
+        <f t="shared" si="1"/>
+        <v>5.4999186393222432E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -669,14 +1843,22 @@
       <c r="C12" s="3">
         <v>39294.65</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="6">
+        <f t="shared" si="0"/>
+        <v>0.31145834505754522</v>
+      </c>
+      <c r="E12" s="3">
         <v>499195.16</v>
       </c>
-      <c r="E12" s="3">
+      <c r="F12" s="3">
         <v>73167.88</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" s="6">
+        <f t="shared" si="1"/>
+        <v>0.14657169352363114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -686,14 +1868,22 @@
       <c r="C13" s="3">
         <v>10493.774600000001</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1064795501442968</v>
+      </c>
+      <c r="E13" s="3">
         <v>41216.58</v>
       </c>
-      <c r="E13" s="3">
+      <c r="F13" s="3">
         <v>6445.97</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13" s="6">
+        <f t="shared" si="1"/>
+        <v>0.15639264587212234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -703,14 +1893,22 @@
       <c r="C14" s="3">
         <v>5427.03</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="6">
+        <f t="shared" si="0"/>
+        <v>0.88435064871576763</v>
+      </c>
+      <c r="E14" s="3">
         <v>101510.56</v>
       </c>
-      <c r="E14" s="3">
+      <c r="F14" s="3">
         <v>3703.44</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G14" s="6">
+        <f t="shared" si="1"/>
+        <v>3.6483297895312565E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -720,14 +1918,22 @@
       <c r="C15" s="3">
         <v>2509.35</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="6">
+        <f t="shared" si="0"/>
+        <v>0.52554804145993594</v>
+      </c>
+      <c r="E15" s="3">
         <v>14520.36</v>
       </c>
-      <c r="E15" s="3">
+      <c r="F15" s="3">
         <v>3334.15</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G15" s="6">
+        <f t="shared" si="1"/>
+        <v>0.22961896261525197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -737,78 +1943,97 @@
       <c r="C16" s="3">
         <v>2508.8200000000002</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="6">
+        <f t="shared" si="0"/>
+        <v>2.3318554870851109</v>
+      </c>
+      <c r="E16" s="3">
         <v>8374.8700000000008</v>
       </c>
-      <c r="E16" s="3">
+      <c r="F16" s="3">
         <v>3108.3</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G16" s="6">
+        <f t="shared" si="1"/>
+        <v>0.3711460595806263</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
     </row>
   </sheetData>
@@ -817,12 +2042,13 @@
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Tests preparados para comparar en la misma maquina
</commit_message>
<xml_diff>
--- a/task-processor-performance/datos/Graficos.xlsx
+++ b/task-processor-performance/datos/Graficos.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Descripción de test</t>
   </si>
@@ -113,6 +113,24 @@
   </si>
   <si>
     <t>Ikari01 (windows32)</t>
+  </si>
+  <si>
+    <t>5 NoSync</t>
+  </si>
+  <si>
+    <t>6 Sync</t>
+  </si>
+  <si>
+    <t>7 NoSync</t>
+  </si>
+  <si>
+    <t>8 Sync</t>
+  </si>
+  <si>
+    <t>IkariNote03 (windows64)</t>
+  </si>
+  <si>
+    <t>IkariNote03(Linux64)</t>
   </si>
 </sst>
 </file>
@@ -177,10 +195,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,7 +258,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejecucion mas rápida'!$B$3:$C$3</c:f>
+              <c:f>'Ejecucion mas rápida'!$F$3:$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -281,7 +299,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ejecucion mas rápida'!$B$6:$B$12</c:f>
+              <c:f>'Ejecucion mas rápida'!$F$6:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -315,7 +333,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejecucion mas rápida'!$E$3:$F$3</c:f>
+              <c:f>'Ejecucion mas rápida'!$I$3:$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -356,7 +374,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ejecucion mas rápida'!$E$6:$E$12</c:f>
+              <c:f>'Ejecucion mas rápida'!$I$6:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -381,6 +399,114 @@
                 <c:pt idx="6">
                   <c:v>499195.16</c:v>
                 </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$B$3:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IkariNote03 (windows64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$6:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SimpleLoopMultiThreadTester x 1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>UnicoThreadALoBruto</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$B$6:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$D$3:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IkariNote03(Linux64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$6:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SimpleLoopMultiThreadTester x 1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>UnicoThreadALoBruto</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$D$6:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="7"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -394,11 +520,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="44424576"/>
-        <c:axId val="78760192"/>
+        <c:axId val="80625024"/>
+        <c:axId val="80635008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44424576"/>
+        <c:axId val="80625024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -417,7 +543,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78760192"/>
+        <c:crossAx val="80635008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -425,7 +551,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78760192"/>
+        <c:axId val="80635008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -436,7 +562,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44424576"/>
+        <c:crossAx val="80625024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -503,7 +629,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejecucion mas rápida'!$B$3:$C$3</c:f>
+              <c:f>'Ejecucion mas rápida'!$F$3:$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -544,7 +670,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ejecucion mas rápida'!$C$6:$C$12</c:f>
+              <c:f>'Ejecucion mas rápida'!$G$6:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -578,7 +704,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejecucion mas rápida'!$E$3:$F$3</c:f>
+              <c:f>'Ejecucion mas rápida'!$I$3:$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -619,7 +745,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ejecucion mas rápida'!$F$6:$F$12</c:f>
+              <c:f>'Ejecucion mas rápida'!$J$6:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -644,6 +770,114 @@
                 <c:pt idx="6">
                   <c:v>73167.88</c:v>
                 </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$B$3:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IkariNote03 (windows64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$6:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SimpleLoopMultiThreadTester x 1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>UnicoThreadALoBruto</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$C$6:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$D$3:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IkariNote03(Linux64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$6:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4X SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2VM x UnicoThreadALoBruto</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SimpleLoopTester</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SimpleLoopMultiThreadTester x 1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>UnicoThreadALoBruto</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$E$6:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="7"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -657,11 +891,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="38571392"/>
-        <c:axId val="85423232"/>
+        <c:axId val="80709504"/>
+        <c:axId val="80711040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="38571392"/>
+        <c:axId val="80709504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -680,7 +914,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85423232"/>
+        <c:crossAx val="80711040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -688,7 +922,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85423232"/>
+        <c:axId val="80711040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,7 +933,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38571392"/>
+        <c:crossAx val="80709504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -766,7 +1000,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejecucion mas rápida'!$B$3:$C$3</c:f>
+              <c:f>'Ejecucion mas rápida'!$F$3:$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -798,7 +1032,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ejecucion mas rápida'!$B$13:$B$16</c:f>
+              <c:f>'Ejecucion mas rápida'!$F$13:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -823,7 +1057,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejecucion mas rápida'!$E$3:$F$3</c:f>
+              <c:f>'Ejecucion mas rápida'!$I$3:$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -855,7 +1089,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ejecucion mas rápida'!$E$13:$E$16</c:f>
+              <c:f>'Ejecucion mas rápida'!$I$13:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -871,6 +1105,96 @@
                 <c:pt idx="3">
                   <c:v>8374.8700000000008</c:v>
                 </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$B$3:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IkariNote03 (windows64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$13:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MultiplesThreadsALoBruto x 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SimpleLoopMultiThreadTester x 4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MultiplesThreadsALoBruto x 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MultiplesThreadsALoBruto x 32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$D$3:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IkariNote03(Linux64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$13:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MultiplesThreadsALoBruto x 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SimpleLoopMultiThreadTester x 4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MultiplesThreadsALoBruto x 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MultiplesThreadsALoBruto x 32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$D$13:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="4"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -884,11 +1208,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="85651840"/>
-        <c:axId val="85654528"/>
+        <c:axId val="81891712"/>
+        <c:axId val="81893248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="85651840"/>
+        <c:axId val="81891712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,7 +1231,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85654528"/>
+        <c:crossAx val="81893248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -915,7 +1239,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85654528"/>
+        <c:axId val="81893248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -926,7 +1250,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85651840"/>
+        <c:crossAx val="81891712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -993,7 +1317,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejecucion mas rápida'!$B$3:$C$3</c:f>
+              <c:f>'Ejecucion mas rápida'!$F$3:$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1025,7 +1349,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ejecucion mas rápida'!$C$13:$C$16</c:f>
+              <c:f>'Ejecucion mas rápida'!$G$13:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1050,7 +1374,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejecucion mas rápida'!$E$3:$F$3</c:f>
+              <c:f>'Ejecucion mas rápida'!$I$3:$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1082,7 +1406,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ejecucion mas rápida'!$F$13:$F$16</c:f>
+              <c:f>'Ejecucion mas rápida'!$J$13:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1098,6 +1422,96 @@
                 <c:pt idx="3">
                   <c:v>3108.3</c:v>
                 </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$B$3:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IkariNote03 (windows64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$13:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MultiplesThreadsALoBruto x 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SimpleLoopMultiThreadTester x 4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MultiplesThreadsALoBruto x 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MultiplesThreadsALoBruto x 32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$C$13:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$D$3:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IkariNote03(Linux64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Ejecucion mas rápida'!$A$13:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MultiplesThreadsALoBruto x 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SimpleLoopMultiThreadTester x 4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MultiplesThreadsALoBruto x 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MultiplesThreadsALoBruto x 32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ejecucion mas rápida'!$E$13:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="4"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1111,11 +1525,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="85627264"/>
-        <c:axId val="85645184"/>
+        <c:axId val="82575744"/>
+        <c:axId val="82577280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="85627264"/>
+        <c:axId val="82575744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1134,7 +1548,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85645184"/>
+        <c:crossAx val="82577280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1142,7 +1556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85645184"/>
+        <c:axId val="82577280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1153,7 +1567,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85627264"/>
+        <c:crossAx val="82575744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1180,13 +1594,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>247651</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>685800</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
@@ -1209,16 +1623,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1242,13 +1656,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:colOff>333376</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:colOff>590551</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1274,15 +1688,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
+      <xdr:colOff>714375</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1593,44 +2007,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G28"/>
+  <dimension ref="A2:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="6"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1641,16 +2065,28 @@
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1660,390 +2096,448 @@
       <c r="C5" s="3">
         <v>0</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
       <c r="E5" s="3">
         <v>0</v>
       </c>
       <c r="F5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
         <v>914424</v>
       </c>
-      <c r="C6" s="3">
+      <c r="G6" s="3">
         <f xml:space="preserve"> 8 * 20127.75</f>
         <v>161022</v>
       </c>
-      <c r="D6" s="6">
-        <f>C6/B6</f>
+      <c r="H6" s="5">
+        <f>G6/F6</f>
         <v>0.17609117870922023</v>
       </c>
-      <c r="E6" s="3">
+      <c r="I6" s="3">
         <f>8 * 589630.29</f>
         <v>4717042.32</v>
       </c>
-      <c r="F6" s="3">
+      <c r="J6" s="3">
         <f xml:space="preserve"> 8 *30953.32</f>
         <v>247626.56</v>
       </c>
-      <c r="G6" s="6">
-        <f>F6/E6</f>
+      <c r="K6" s="5">
+        <f>J6/I6</f>
         <v>5.2496149748344843E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
         <f>4 * 194176.23</f>
         <v>776704.92</v>
       </c>
-      <c r="C7" s="3">
+      <c r="G7" s="3">
         <f>4 * 37921.61</f>
         <v>151686.44</v>
       </c>
-      <c r="D7" s="6">
-        <f t="shared" ref="D7:D16" si="0">C7/B7</f>
+      <c r="H7" s="5">
+        <f t="shared" ref="H7:H16" si="0">G7/F7</f>
         <v>0.19529481028651138</v>
       </c>
-      <c r="E7" s="3">
+      <c r="I7" s="3">
         <f xml:space="preserve"> 4 *944117.5</f>
         <v>3776470</v>
       </c>
-      <c r="F7" s="3">
+      <c r="J7" s="3">
         <f>4 * 60614.82</f>
         <v>242459.28</v>
       </c>
-      <c r="G7" s="6">
-        <f t="shared" ref="G7:G16" si="1">F7/E7</f>
+      <c r="K7" s="5">
+        <f t="shared" ref="K7:K16" si="1">J7/I7</f>
         <v>6.4202623084520724E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
         <f>4*125486.01</f>
         <v>501944.04</v>
       </c>
-      <c r="C8" s="3">
+      <c r="G8" s="3">
         <f>4 * 38627.17</f>
         <v>154508.68</v>
       </c>
-      <c r="D8" s="6">
+      <c r="H8" s="5">
         <f t="shared" si="0"/>
         <v>0.30782052915699526</v>
       </c>
-      <c r="E8" s="3">
+      <c r="I8" s="3">
         <f>4 * 466324.96</f>
         <v>1865299.84</v>
       </c>
-      <c r="F8" s="3">
+      <c r="J8" s="3">
         <f>4 * 41314.08</f>
         <v>165256.32000000001</v>
       </c>
-      <c r="G8" s="6">
+      <c r="K8" s="5">
         <f t="shared" si="1"/>
         <v>8.8595043250526417E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
         <f>2*125605.79</f>
         <v>251211.58</v>
       </c>
-      <c r="C9" s="3">
+      <c r="G9" s="3">
         <f>2 * 39277.56</f>
         <v>78555.12</v>
       </c>
-      <c r="D9" s="6">
+      <c r="H9" s="5">
         <f t="shared" si="0"/>
         <v>0.31270501144891488</v>
       </c>
-      <c r="E9" s="3">
+      <c r="I9" s="3">
         <f>2*489983.22</f>
         <v>979966.44</v>
       </c>
-      <c r="F9" s="3">
+      <c r="J9" s="3">
         <f xml:space="preserve"> 2 * 70314.33</f>
         <v>140628.66</v>
       </c>
-      <c r="G9" s="6">
+      <c r="K9" s="5">
         <f t="shared" si="1"/>
         <v>0.14350354691738221</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
         <v>194494.19</v>
       </c>
-      <c r="C10" s="3">
+      <c r="G10" s="3">
         <v>38212.33</v>
       </c>
-      <c r="D10" s="6">
+      <c r="H10" s="5">
         <f t="shared" si="0"/>
         <v>0.19647029044929312</v>
       </c>
-      <c r="E10" s="3">
+      <c r="I10" s="3">
         <v>1237362.42</v>
       </c>
-      <c r="F10" s="3">
+      <c r="J10" s="3">
         <v>69191.94</v>
       </c>
-      <c r="G10" s="6">
+      <c r="K10" s="5">
         <f t="shared" si="1"/>
         <v>5.5918895613461417E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
         <v>156932.69</v>
       </c>
-      <c r="C11" s="3">
+      <c r="G11" s="3">
         <v>37754.9</v>
       </c>
-      <c r="D11" s="6">
+      <c r="H11" s="5">
         <f t="shared" si="0"/>
         <v>0.24058021308371125</v>
       </c>
-      <c r="E11" s="3">
+      <c r="I11" s="3">
         <v>1234625.8999999999</v>
       </c>
-      <c r="F11" s="3">
+      <c r="J11" s="3">
         <v>67903.42</v>
       </c>
-      <c r="G11" s="6">
+      <c r="K11" s="5">
         <f t="shared" si="1"/>
         <v>5.4999186393222432E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3">
         <v>126163.42</v>
       </c>
-      <c r="C12" s="3">
+      <c r="G12" s="3">
         <v>39294.65</v>
       </c>
-      <c r="D12" s="6">
+      <c r="H12" s="5">
         <f t="shared" si="0"/>
         <v>0.31145834505754522</v>
       </c>
-      <c r="E12" s="3">
+      <c r="I12" s="3">
         <v>499195.16</v>
       </c>
-      <c r="F12" s="3">
+      <c r="J12" s="3">
         <v>73167.88</v>
       </c>
-      <c r="G12" s="6">
+      <c r="K12" s="5">
         <f t="shared" si="1"/>
         <v>0.14657169352363114</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
         <v>9483.93</v>
       </c>
-      <c r="C13" s="3">
+      <c r="G13" s="3">
         <v>10493.774600000001</v>
       </c>
-      <c r="D13" s="6">
+      <c r="H13" s="5">
         <f t="shared" si="0"/>
         <v>1.1064795501442968</v>
       </c>
-      <c r="E13" s="3">
+      <c r="I13" s="3">
         <v>41216.58</v>
       </c>
-      <c r="F13" s="3">
+      <c r="J13" s="3">
         <v>6445.97</v>
       </c>
-      <c r="G13" s="6">
+      <c r="K13" s="5">
         <f t="shared" si="1"/>
         <v>0.15639264587212234</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3">
         <v>6136.74</v>
       </c>
-      <c r="C14" s="3">
+      <c r="G14" s="3">
         <v>5427.03</v>
       </c>
-      <c r="D14" s="6">
+      <c r="H14" s="5">
         <f t="shared" si="0"/>
         <v>0.88435064871576763</v>
       </c>
-      <c r="E14" s="3">
+      <c r="I14" s="3">
         <v>101510.56</v>
       </c>
-      <c r="F14" s="3">
+      <c r="J14" s="3">
         <v>3703.44</v>
       </c>
-      <c r="G14" s="6">
+      <c r="K14" s="5">
         <f t="shared" si="1"/>
         <v>3.6483297895312565E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3">
         <v>4774.7299999999996</v>
       </c>
-      <c r="C15" s="3">
+      <c r="G15" s="3">
         <v>2509.35</v>
       </c>
-      <c r="D15" s="6">
+      <c r="H15" s="5">
         <f t="shared" si="0"/>
         <v>0.52554804145993594</v>
       </c>
-      <c r="E15" s="3">
+      <c r="I15" s="3">
         <v>14520.36</v>
       </c>
-      <c r="F15" s="3">
+      <c r="J15" s="3">
         <v>3334.15</v>
       </c>
-      <c r="G15" s="6">
+      <c r="K15" s="5">
         <f t="shared" si="1"/>
         <v>0.22961896261525197</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3">
         <v>1075.8900000000001</v>
       </c>
-      <c r="C16" s="3">
+      <c r="G16" s="3">
         <v>2508.8200000000002</v>
       </c>
-      <c r="D16" s="6">
+      <c r="H16" s="5">
         <f t="shared" si="0"/>
         <v>2.3318554870851109</v>
       </c>
-      <c r="E16" s="3">
+      <c r="I16" s="3">
         <v>8374.8700000000008</v>
       </c>
-      <c r="F16" s="3">
+      <c r="J16" s="3">
         <v>3108.3</v>
       </c>
-      <c r="G16" s="6">
+      <c r="K16" s="5">
         <f t="shared" si="1"/>
         <v>0.3711460595806263</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F28" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A6:C16">
-    <sortCondition descending="1" ref="B6:B16"/>
+  <sortState ref="A6:G16">
+    <sortCondition descending="1" ref="F6:F16"/>
   </sortState>
-  <mergeCells count="3">
+  <mergeCells count="5">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Dato corregido al excel
</commit_message>
<xml_diff>
--- a/task-processor-performance/datos/Graficos.xlsx
+++ b/task-processor-performance/datos/Graficos.xlsx
@@ -322,7 +322,7 @@
                   <c:v>156932.69</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>126163.42</c:v>
+                  <c:v>269281.94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -520,11 +520,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="80625024"/>
-        <c:axId val="80635008"/>
+        <c:axId val="79262848"/>
+        <c:axId val="79264384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80625024"/>
+        <c:axId val="79262848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -543,7 +543,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80635008"/>
+        <c:crossAx val="79264384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -551,7 +551,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80635008"/>
+        <c:axId val="79264384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,7 +562,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80625024"/>
+        <c:crossAx val="79262848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -891,11 +891,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="80709504"/>
-        <c:axId val="80711040"/>
+        <c:axId val="79508608"/>
+        <c:axId val="79510144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80709504"/>
+        <c:axId val="79508608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -914,7 +914,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80711040"/>
+        <c:crossAx val="79510144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -922,7 +922,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80711040"/>
+        <c:axId val="79510144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -933,7 +933,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80709504"/>
+        <c:crossAx val="79508608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1208,11 +1208,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="81891712"/>
-        <c:axId val="81893248"/>
+        <c:axId val="79553664"/>
+        <c:axId val="79555200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81891712"/>
+        <c:axId val="79553664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1231,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81893248"/>
+        <c:crossAx val="79555200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1239,7 +1239,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81893248"/>
+        <c:axId val="79555200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,7 +1250,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81891712"/>
+        <c:crossAx val="79553664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1525,11 +1525,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82575744"/>
-        <c:axId val="82577280"/>
+        <c:axId val="82334848"/>
+        <c:axId val="82336384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82575744"/>
+        <c:axId val="82334848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1548,7 +1548,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82577280"/>
+        <c:crossAx val="82336384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1556,7 +1556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82577280"/>
+        <c:axId val="82336384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1567,7 +1567,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82575744"/>
+        <c:crossAx val="82334848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2010,7 +2010,7 @@
   <dimension ref="A2:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,14 +2314,14 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3">
-        <v>126163.42</v>
+        <v>269281.94</v>
       </c>
       <c r="G12" s="3">
         <v>39294.65</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="0"/>
-        <v>0.31145834505754522</v>
+        <v>0.14592382244423818</v>
       </c>
       <c r="I12" s="3">
         <v>499195.16</v>

</xml_diff>

<commit_message>
Datos de windows note03
</commit_message>
<xml_diff>
--- a/task-processor-performance/datos/Graficos.xlsx
+++ b/task-processor-performance/datos/Graficos.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Docs\Git\vortex\task-processor-performance\datos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="9570" windowHeight="9780"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -21,7 +26,7 @@
     <author>ikari</author>
   </authors>
   <commentList>
-    <comment ref="A6" authorId="0">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -209,6 +214,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -216,7 +224,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -453,6 +461,27 @@
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3010551.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2341189.6800000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1072594.52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>441362.84</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>588878.35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>594142.91</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200044.69</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -520,16 +549,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="79262848"/>
-        <c:axId val="79264384"/>
+        <c:axId val="244952008"/>
+        <c:axId val="196836368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="79262848"/>
+        <c:axId val="244952008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -543,7 +573,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79264384"/>
+        <c:crossAx val="196836368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -551,7 +581,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79264384"/>
+        <c:axId val="196836368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,7 +592,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79262848"/>
+        <c:crossAx val="244952008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -587,7 +617,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -891,16 +921,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="79508608"/>
-        <c:axId val="79510144"/>
+        <c:axId val="196837152"/>
+        <c:axId val="197504336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="79508608"/>
+        <c:axId val="196837152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -914,7 +945,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79510144"/>
+        <c:crossAx val="197504336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -922,7 +953,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79510144"/>
+        <c:axId val="197504336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -933,7 +964,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79508608"/>
+        <c:crossAx val="196837152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -958,7 +989,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1150,6 +1181,18 @@
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>203012.79</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>455707.54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>126068.81</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>119128.89</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1208,16 +1251,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="79553664"/>
-        <c:axId val="79555200"/>
+        <c:axId val="197505904"/>
+        <c:axId val="197506296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="79553664"/>
+        <c:axId val="197505904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1231,7 +1275,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79555200"/>
+        <c:crossAx val="197506296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1239,7 +1283,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79555200"/>
+        <c:axId val="197506296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,7 +1294,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79553664"/>
+        <c:crossAx val="197505904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1275,7 +1319,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1525,16 +1569,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82334848"/>
-        <c:axId val="82336384"/>
+        <c:axId val="197504728"/>
+        <c:axId val="197507080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82334848"/>
+        <c:axId val="197504728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1548,7 +1593,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82336384"/>
+        <c:crossAx val="197507080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1556,7 +1601,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82336384"/>
+        <c:axId val="197507080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1567,7 +1612,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82334848"/>
+        <c:crossAx val="197504728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1721,7 +1766,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1763,7 +1808,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1798,7 +1843,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2010,10 +2055,10 @@
   <dimension ref="A2:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="11.7109375" customWidth="1"/>
@@ -2120,7 +2165,10 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3">
+        <f>8 *376318.99</f>
+        <v>3010551.92</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -2152,7 +2200,10 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="3">
+        <f>4 * 585297.42</f>
+        <v>2341189.6800000002</v>
+      </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -2185,7 +2236,10 @@
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3">
+        <f xml:space="preserve"> 4 * 268148.63</f>
+        <v>1072594.52</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -2218,7 +2272,10 @@
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3">
+        <f>2*220681.42</f>
+        <v>441362.84</v>
+      </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -2251,7 +2308,9 @@
       <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3">
+        <v>588878.35</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -2280,7 +2339,9 @@
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3">
+        <v>594142.91</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -2309,7 +2370,9 @@
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3">
+        <v>200044.69</v>
+      </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -2338,7 +2401,9 @@
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="3">
+        <v>203012.79</v>
+      </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -2367,7 +2432,9 @@
       <c r="A14" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="3">
+        <v>455707.54</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -2396,7 +2463,9 @@
       <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="3">
+        <v>126068.81</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2425,7 +2494,9 @@
       <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="3">
+        <v>119128.89</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -2552,7 +2623,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2564,7 +2635,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>